<commit_message>
final added with model 1
</commit_message>
<xml_diff>
--- a/831MarketingAnalytics/Project/831MarketingProject/output/cluster_summary.xlsx
+++ b/831MarketingAnalytics/Project/831MarketingProject/output/cluster_summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,88 +441,108 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Loan Amount</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Outstanding Balance</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Interest Rate</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Loan Term (Months)</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Stated Income on application</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Qualified / Verified
 Income</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Aptitude for change Score</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Financial Literacy Score</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Self Assessments</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Mood Count</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Average total activities per month</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Debt_to_Income_Ratio</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Remaining_Loan_Percentage</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Loan_to_Income_Ratio</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Consistency_Score</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Remaining_Tenure</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Activity_Diversity</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Missed_Periods</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Cluster</t>
         </is>
       </c>
     </row>
@@ -531,55 +551,67 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>13507.54606741573</v>
+        <v>11322.875</v>
       </c>
       <c r="C2" t="n">
-        <v>18563.77561797753</v>
+        <v>15034.73375</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2854056179775281</v>
+        <v>19803.4025</v>
       </c>
       <c r="E2" t="n">
-        <v>55.92134831460674</v>
+        <v>0.2862888888888889</v>
       </c>
       <c r="F2" t="n">
-        <v>70586.17977528089</v>
+        <v>56.41666666666666</v>
       </c>
       <c r="G2" t="n">
-        <v>68318.32584269663</v>
+        <v>76854.97222222222</v>
       </c>
       <c r="H2" t="n">
-        <v>3.27876404494382</v>
+        <v>73894.44444444444</v>
       </c>
       <c r="I2" t="n">
-        <v>2.393258426966292</v>
+        <v>3.266388888888889</v>
       </c>
       <c r="J2" t="n">
-        <v>5.617977528089888</v>
+        <v>2.472222222222222</v>
       </c>
       <c r="K2" t="n">
-        <v>4.269662921348314</v>
+        <v>6.597222222222222</v>
       </c>
       <c r="L2" t="n">
-        <v>4.458716853932584</v>
+        <v>4.736111111111111</v>
       </c>
       <c r="M2" t="n">
-        <v>0.1741518095358089</v>
+        <v>4.639168055555555</v>
       </c>
       <c r="N2" t="n">
-        <v>1.331179232571444</v>
+        <v>0.1737996459739308</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2155897608076222</v>
+        <v>1.319563417002594</v>
       </c>
       <c r="P2" t="n">
-        <v>0.02171828728889261</v>
+        <v>0.2163854196655239</v>
       </c>
       <c r="Q2" t="n">
-        <v>30.76404494382022</v>
+        <v>0.02314480320969429</v>
       </c>
       <c r="R2" t="n">
-        <v>42.43820224719101</v>
+        <v>36.86111111111111</v>
+      </c>
+      <c r="S2" t="n">
+        <v>40.90277777777778</v>
+      </c>
+      <c r="T2" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.5763151622395932</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -587,55 +619,67 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>15888.31222222222</v>
+        <v>11186.34426229508</v>
       </c>
       <c r="C3" t="n">
-        <v>18570.34388888889</v>
+        <v>15970.45180327869</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2787888888888889</v>
+        <v>20409.88508196721</v>
       </c>
       <c r="E3" t="n">
-        <v>54.94444444444444</v>
+        <v>0.2838344262295082</v>
       </c>
       <c r="F3" t="n">
-        <v>92272.63888888889</v>
+        <v>57.01639344262295</v>
       </c>
       <c r="G3" t="n">
-        <v>73975</v>
+        <v>77559.40983606558</v>
       </c>
       <c r="H3" t="n">
-        <v>2.773055555555556</v>
+        <v>87053.27868852459</v>
       </c>
       <c r="I3" t="n">
-        <v>1.833333333333333</v>
+        <v>3.177540983606558</v>
       </c>
       <c r="J3" t="n">
-        <v>8.861111111111111</v>
+        <v>2.868852459016393</v>
       </c>
       <c r="K3" t="n">
-        <v>17.69444444444444</v>
+        <v>8.836065573770492</v>
       </c>
       <c r="L3" t="n">
-        <v>5.307444444444445</v>
+        <v>7.655737704918033</v>
       </c>
       <c r="M3" t="n">
-        <v>0.1669524304070877</v>
+        <v>6.390165573770491</v>
       </c>
       <c r="N3" t="n">
-        <v>1.199024322517959</v>
+        <v>0.1618202756124067</v>
       </c>
       <c r="O3" t="n">
-        <v>0.230496671095215</v>
+        <v>1.285643004620153</v>
       </c>
       <c r="P3" t="n">
-        <v>0.02311147316544034</v>
+        <v>0.2121999110056152</v>
       </c>
       <c r="Q3" t="n">
-        <v>57.80555555555556</v>
+        <v>0.02622901379365879</v>
       </c>
       <c r="R3" t="n">
-        <v>35.91666666666666</v>
+        <v>46.9344262295082</v>
+      </c>
+      <c r="S3" t="n">
+        <v>41.29508196721311</v>
+      </c>
+      <c r="T3" t="n">
+        <v>1.80327868852459</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.6734740569407228</v>
+      </c>
+      <c r="V3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -643,55 +687,135 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>15584.92287356322</v>
+        <v>8555.448275862069</v>
       </c>
       <c r="C4" t="n">
-        <v>20297.39459770115</v>
+        <v>15814.80137931034</v>
       </c>
       <c r="D4" t="n">
-        <v>0.2849574712643678</v>
+        <v>19380.13793103448</v>
       </c>
       <c r="E4" t="n">
-        <v>57.36781609195403</v>
+        <v>0.2774862068965517</v>
       </c>
       <c r="F4" t="n">
-        <v>76569.14942528735</v>
+        <v>54.44827586206897</v>
       </c>
       <c r="G4" t="n">
-        <v>81562.64367816092</v>
+        <v>95960.44827586207</v>
       </c>
       <c r="H4" t="n">
-        <v>3.316206896551724</v>
+        <v>72451.72413793103</v>
       </c>
       <c r="I4" t="n">
-        <v>2.862068965517242</v>
+        <v>3.114827586206896</v>
       </c>
       <c r="J4" t="n">
-        <v>8.080459770114942</v>
+        <v>1.931034482758621</v>
       </c>
       <c r="K4" t="n">
-        <v>6.563218390804598</v>
+        <v>8.793103448275861</v>
       </c>
       <c r="L4" t="n">
-        <v>5.99103908045977</v>
+        <v>19.06896551724138</v>
       </c>
       <c r="M4" t="n">
-        <v>0.1696744584511038</v>
+        <v>5.428810344827586</v>
       </c>
       <c r="N4" t="n">
-        <v>1.304445508474827</v>
+        <v>0.1802418272197341</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2143518471829714</v>
+        <v>1.225321512882849</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0260557931824584</v>
+        <v>0.233650954215871</v>
       </c>
       <c r="Q4" t="n">
-        <v>43.74712643678161</v>
+        <v>0.02294853230255155</v>
       </c>
       <c r="R4" t="n">
-        <v>42.0919540229885</v>
+        <v>59.20689655172414</v>
+      </c>
+      <c r="S4" t="n">
+        <v>35.41379310344828</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1.586206896551724</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.5596866509069731</v>
+      </c>
+      <c r="V4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>13751.18</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12294.23</v>
+      </c>
+      <c r="D5" t="n">
+        <v>17074.1954</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2851</v>
+      </c>
+      <c r="F5" t="n">
+        <v>56.54</v>
+      </c>
+      <c r="G5" t="n">
+        <v>64359.32</v>
+      </c>
+      <c r="H5" t="n">
+        <v>62152.62</v>
+      </c>
+      <c r="I5" t="n">
+        <v>3.2162</v>
+      </c>
+      <c r="J5" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="K5" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="L5" t="n">
+        <v>4.54</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4.55717</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1731970423347213</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1.323189467343925</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.2166831423340825</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.02199783000512013</v>
+      </c>
+      <c r="R5" t="n">
+        <v>27.82</v>
+      </c>
+      <c r="S5" t="n">
+        <v>44.82</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.6121051984050072</v>
+      </c>
+      <c r="V5" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>